<commit_message>
index modified for thesis april 2024
</commit_message>
<xml_diff>
--- a/theses/2024april/responses.xlsx
+++ b/theses/2024april/responses.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/claragarciasan/Documents/TUDelft/GitRepos/geo2020/theses/2024april/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1C3B0B1-BDC8-1048-910F-4702F936D8A2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24368BD8-38D0-E140-B504-39B0C7D0D03C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="30240" yWindow="500" windowWidth="38400" windowHeight="21100" tabRatio="204" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17020" tabRatio="204" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="WaB3blYZ" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="88">
   <si>
     <t>#</t>
   </si>
@@ -288,15 +288,33 @@
   <si>
     <t>08635d5430</t>
   </si>
+  <si>
+    <t>Solar potential analysis is of great help to energy transition through city planning, analysis of
+occupant behavior, assessing building energy performance, and scheduling the power grid.
+Computing high resolution (spatial, temporal, and semantic) solar irradiance is the key step
+of solar potential analysis. To determine the solar irradiance with high resolution, we can
+utilize 3D City Models (3DCM). Within the context of 3DCM, calculating shadows, sky-view
+factor (SVF), and ground view factor (GVF) are the most important and computationally
+intensive steps. Existing methods for the calculations, either apply simplifications or
+assumptions to make the computation achievable in a limited time. While some methods are
+accurate, but unable to scale to city-level. The thesis will be focused on developing a
+methodology that can achieve fast shadow solar irradiance with minimum assumptions. The
+expected methodology will be able to be applied to large areas such as the whole Netherlands</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -319,9 +337,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -664,12 +685,14 @@
   <dimension ref="A1:R6"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A5" activeCellId="1" sqref="A3:XFD3 A5:XFD5"/>
+      <selection activeCell="I7" sqref="I7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="15" width="9.5" style="1"/>
+    <col min="1" max="8" width="9.5" style="1"/>
+    <col min="9" max="9" width="255.83203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="15" width="9.5" style="1"/>
     <col min="16" max="16" width="18.1640625" style="1" bestFit="1" customWidth="1"/>
     <col min="17" max="18" width="9.5" style="1"/>
   </cols>
@@ -954,7 +977,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:18" ht="409.6" x14ac:dyDescent="0.15">
       <c r="A6" s="1" t="s">
         <v>74</v>
       </c>
@@ -979,8 +1002,8 @@
       <c r="H6" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="I6" s="1" t="s">
-        <v>78</v>
+      <c r="I6" s="2" t="s">
+        <v>87</v>
       </c>
       <c r="J6" s="1" t="s">
         <v>81</v>

</xml_diff>